<commit_message>
Updated variables of interest excel
</commit_message>
<xml_diff>
--- a/Variables_of_Interest.xlsx
+++ b/Variables_of_Interest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katni\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C880E7-DB72-4031-9B0F-8272F118B65D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895562BE-EB09-4E36-A297-93E43E7DA019}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2205" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-1545" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcome Variables" sheetId="2" r:id="rId1"/>
@@ -565,7 +565,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9167" uniqueCount="2005">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9167" uniqueCount="2004">
   <si>
     <t>Wave I</t>
   </si>
@@ -6508,9 +6508,6 @@
   </si>
   <si>
     <t>Location</t>
-  </si>
-  <si>
-    <t>Variable</t>
   </si>
   <si>
     <t>Variable Description</t>
@@ -10305,8 +10302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC527C8-F3E3-4E08-93D4-30E7EF640FEC}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10316,7 +10313,7 @@
     <col min="3" max="3" width="10" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -10325,7 +10322,7 @@
         <v>1980</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1472</v>
@@ -10337,7 +10334,7 @@
         <v>1410</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>1981</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -10569,7 +10566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E91241-5C1E-AE4D-8583-A4D88238CB65}">
   <dimension ref="A1:AB63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="R37" sqref="R37"/>
     </sheetView>
@@ -12522,7 +12519,7 @@
     </row>
     <row r="47" spans="1:28" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="78" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="B47" s="87"/>
       <c r="C47" s="87"/>
@@ -13730,7 +13727,7 @@
         <v>1964</v>
       </c>
       <c r="C15" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D15" s="80" t="s">
         <v>553</v>
@@ -13756,7 +13753,7 @@
         <v>1964</v>
       </c>
       <c r="C16" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D16" s="80" t="s">
         <v>559</v>
@@ -13782,7 +13779,7 @@
         <v>1964</v>
       </c>
       <c r="C17" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D17" s="80" t="s">
         <v>562</v>
@@ -13808,7 +13805,7 @@
         <v>1964</v>
       </c>
       <c r="C18" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D18" s="80" t="s">
         <v>564</v>
@@ -13834,7 +13831,7 @@
         <v>1964</v>
       </c>
       <c r="C19" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D19" s="80" t="s">
         <v>567</v>
@@ -13860,7 +13857,7 @@
         <v>1964</v>
       </c>
       <c r="C20" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D20" s="80" t="s">
         <v>569</v>
@@ -13886,7 +13883,7 @@
         <v>1964</v>
       </c>
       <c r="C21" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D21" s="80" t="s">
         <v>575</v>
@@ -13912,7 +13909,7 @@
         <v>1964</v>
       </c>
       <c r="C22" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D22" s="80" t="s">
         <v>581</v>
@@ -13938,7 +13935,7 @@
         <v>1964</v>
       </c>
       <c r="C23" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D23" s="80" t="s">
         <v>587</v>
@@ -13964,7 +13961,7 @@
         <v>1964</v>
       </c>
       <c r="C24" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D24" s="80" t="s">
         <v>591</v>
@@ -13990,7 +13987,7 @@
         <v>1964</v>
       </c>
       <c r="C25" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D25" s="80" t="s">
         <v>597</v>
@@ -14016,7 +14013,7 @@
         <v>1964</v>
       </c>
       <c r="C26" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D26" s="80" t="s">
         <v>603</v>
@@ -14380,7 +14377,7 @@
         <v>1950</v>
       </c>
       <c r="C40" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D40" s="80" t="s">
         <v>553</v>
@@ -14406,7 +14403,7 @@
         <v>1950</v>
       </c>
       <c r="C41" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D41" s="80" t="s">
         <v>559</v>
@@ -14432,7 +14429,7 @@
         <v>1950</v>
       </c>
       <c r="C42" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D42" s="80" t="s">
         <v>569</v>
@@ -14458,7 +14455,7 @@
         <v>1950</v>
       </c>
       <c r="C43" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D43" s="80" t="s">
         <v>575</v>
@@ -14484,7 +14481,7 @@
         <v>1950</v>
       </c>
       <c r="C44" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D44" s="80" t="s">
         <v>581</v>
@@ -14510,7 +14507,7 @@
         <v>1950</v>
       </c>
       <c r="C45" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D45" s="80" t="s">
         <v>587</v>
@@ -14536,7 +14533,7 @@
         <v>1950</v>
       </c>
       <c r="C46" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D46" s="80" t="s">
         <v>591</v>
@@ -14562,7 +14559,7 @@
         <v>1950</v>
       </c>
       <c r="C47" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D47" s="80" t="s">
         <v>597</v>
@@ -14588,7 +14585,7 @@
         <v>1950</v>
       </c>
       <c r="C48" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D48" s="80" t="s">
         <v>603</v>
@@ -15524,7 +15521,7 @@
         <v>1951</v>
       </c>
       <c r="C84" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D84" s="80" t="s">
         <v>553</v>
@@ -15550,7 +15547,7 @@
         <v>1951</v>
       </c>
       <c r="C85" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D85" s="80" t="s">
         <v>569</v>
@@ -15576,7 +15573,7 @@
         <v>1951</v>
       </c>
       <c r="C86" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D86" s="80" t="s">
         <v>575</v>
@@ -15602,7 +15599,7 @@
         <v>1951</v>
       </c>
       <c r="C87" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D87" s="80" t="s">
         <v>581</v>
@@ -15628,7 +15625,7 @@
         <v>1951</v>
       </c>
       <c r="C88" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D88" s="80" t="s">
         <v>591</v>
@@ -15654,7 +15651,7 @@
         <v>1951</v>
       </c>
       <c r="C89" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D89" s="80" t="s">
         <v>597</v>
@@ -15680,7 +15677,7 @@
         <v>1951</v>
       </c>
       <c r="C90" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D90" s="80" t="s">
         <v>603</v>
@@ -15706,7 +15703,7 @@
         <v>1951</v>
       </c>
       <c r="C91" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D91" s="80" t="s">
         <v>607</v>
@@ -16252,7 +16249,7 @@
         <v>1955</v>
       </c>
       <c r="C112" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D112" s="80" t="s">
         <v>553</v>
@@ -16278,7 +16275,7 @@
         <v>1955</v>
       </c>
       <c r="C113" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D113" s="80" t="s">
         <v>569</v>
@@ -16304,7 +16301,7 @@
         <v>1955</v>
       </c>
       <c r="C114" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D114" s="80" t="s">
         <v>575</v>
@@ -16330,7 +16327,7 @@
         <v>1955</v>
       </c>
       <c r="C115" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D115" s="80" t="s">
         <v>581</v>
@@ -16356,7 +16353,7 @@
         <v>1955</v>
       </c>
       <c r="C116" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D116" s="80" t="s">
         <v>596</v>
@@ -16382,7 +16379,7 @@
         <v>1955</v>
       </c>
       <c r="C117" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D117" s="80" t="s">
         <v>597</v>
@@ -16408,7 +16405,7 @@
         <v>1955</v>
       </c>
       <c r="C118" s="82" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D118" s="80" t="s">
         <v>609</v>
@@ -16456,7 +16453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3F7A32-2A24-9143-AA8A-5502F5BABBAF}">
   <dimension ref="A1:AB230"/>
   <sheetViews>
-    <sheetView topLeftCell="A220" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B166" sqref="B166"/>
     </sheetView>
@@ -38426,7 +38423,7 @@
         <v>1411</v>
       </c>
       <c r="F251" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.25">
@@ -38446,7 +38443,7 @@
         <v>1411</v>
       </c>
       <c r="F252" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.25">
@@ -38466,7 +38463,7 @@
         <v>1411</v>
       </c>
       <c r="F253" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.25">
@@ -38486,7 +38483,7 @@
         <v>1411</v>
       </c>
       <c r="F254" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="255" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -38506,7 +38503,7 @@
         <v>1411</v>
       </c>
       <c r="F255" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="256" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -38526,7 +38523,7 @@
         <v>1411</v>
       </c>
       <c r="F256" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.25">
@@ -38546,7 +38543,7 @@
         <v>1411</v>
       </c>
       <c r="F257" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.25">
@@ -38566,7 +38563,7 @@
         <v>1411</v>
       </c>
       <c r="F258" t="s">
-        <v>1990</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.25">
@@ -38586,7 +38583,7 @@
         <v>1411</v>
       </c>
       <c r="F259" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.25">
@@ -38606,7 +38603,7 @@
         <v>1411</v>
       </c>
       <c r="F260" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="261" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -38626,7 +38623,7 @@
         <v>1411</v>
       </c>
       <c r="F261" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="262" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -38646,7 +38643,7 @@
         <v>1411</v>
       </c>
       <c r="F262" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="263" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -40786,7 +40783,7 @@
         <v>1411</v>
       </c>
       <c r="F369" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="370" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -40806,7 +40803,7 @@
         <v>1411</v>
       </c>
       <c r="F370" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="371" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -40826,7 +40823,7 @@
         <v>1411</v>
       </c>
       <c r="F371" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="372" spans="1:6" x14ac:dyDescent="0.25">
@@ -40846,7 +40843,7 @@
         <v>1411</v>
       </c>
       <c r="F372" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="373" spans="1:6" x14ac:dyDescent="0.25">
@@ -40866,7 +40863,7 @@
         <v>1411</v>
       </c>
       <c r="F373" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="374" spans="1:6" x14ac:dyDescent="0.25">
@@ -40886,7 +40883,7 @@
         <v>1411</v>
       </c>
       <c r="F374" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="375" spans="1:6" x14ac:dyDescent="0.25">
@@ -40906,7 +40903,7 @@
         <v>1411</v>
       </c>
       <c r="F375" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="376" spans="1:6" x14ac:dyDescent="0.25">
@@ -40926,7 +40923,7 @@
         <v>1411</v>
       </c>
       <c r="F376" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="377" spans="1:6" x14ac:dyDescent="0.25">
@@ -40946,7 +40943,7 @@
         <v>1411</v>
       </c>
       <c r="F377" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="378" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates excel file to include heavy drinking variable outcomes
</commit_message>
<xml_diff>
--- a/Variables_of_Interest.xlsx
+++ b/Variables_of_Interest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katni\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895562BE-EB09-4E36-A297-93E43E7DA019}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6769A3E4-BE78-4B4B-B0BE-9EF06D97F291}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1545" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcome Variables" sheetId="2" r:id="rId1"/>
@@ -565,7 +565,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9167" uniqueCount="2004">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9195" uniqueCount="2008">
   <si>
     <t>Wave I</t>
   </si>
@@ -6577,6 +6577,18 @@
   </si>
   <si>
     <t>Behavioral Despair</t>
+  </si>
+  <si>
+    <t>h5to11</t>
+  </si>
+  <si>
+    <t>Have you ever had a drink of beer, wine, or liquor?</t>
+  </si>
+  <si>
+    <t>What sex were you assigned at birth, on your original birth certificate?</t>
+  </si>
+  <si>
+    <t>h5od2a</t>
   </si>
 </sst>
 </file>
@@ -6661,7 +6673,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
@@ -7015,6 +7027,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7501,8 +7514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q83"/>
   <sheetViews>
-    <sheetView zoomScale="88" workbookViewId="0">
-      <selection activeCell="N83" sqref="N83"/>
+    <sheetView topLeftCell="B1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10300,10 +10313,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC527C8-F3E3-4E08-93D4-30E7EF640FEC}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10312,7 +10325,7 @@
     <col min="2" max="2" width="68.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
@@ -10555,6 +10568,100 @@
       </c>
       <c r="F13" s="6" t="s">
         <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="58" t="s">
+        <v>1955</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>1519</v>
+      </c>
+      <c r="D14" s="55" t="s">
+        <v>1407</v>
+      </c>
+      <c r="E14" s="55" t="s">
+        <v>1409</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="58" t="s">
+        <v>1955</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>1519</v>
+      </c>
+      <c r="D15" s="55" t="s">
+        <v>1407</v>
+      </c>
+      <c r="E15" s="55" t="s">
+        <v>1409</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="58" t="s">
+        <v>1955</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>1495</v>
+      </c>
+      <c r="D16" s="55" t="s">
+        <v>1408</v>
+      </c>
+      <c r="E16" s="55" t="s">
+        <v>1411</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="58" t="s">
+        <v>1955</v>
+      </c>
+      <c r="B17" s="126" t="s">
+        <v>2005</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>1474</v>
+      </c>
+      <c r="E17" s="57" t="s">
+        <v>1409</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="58" t="s">
+        <v>1955</v>
+      </c>
+      <c r="B18" s="126" t="s">
+        <v>2006</v>
+      </c>
+      <c r="C18" s="127" t="s">
+        <v>1498</v>
+      </c>
+      <c r="E18" s="57" t="s">
+        <v>1409</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>2007</v>
       </c>
     </row>
   </sheetData>
@@ -13339,7 +13446,7 @@
   <dimension ref="A1:H124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adds descriptor vars to sheet 4, recodes them to factors not numeric
</commit_message>
<xml_diff>
--- a/Variables_of_Interest.xlsx
+++ b/Variables_of_Interest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katni\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E1A65E-0784-492D-81D4-0A212E7CFA65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DB7162-3026-412B-BA9A-ACDE6C725BE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcome Variables" sheetId="2" r:id="rId1"/>
@@ -566,7 +566,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9436" uniqueCount="2050">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9450" uniqueCount="2054">
   <si>
     <t>Wave I</t>
   </si>
@@ -6716,6 +6716,18 @@
   </si>
   <si>
     <t>H5HTENJC</t>
+  </si>
+  <si>
+    <t>Demographic</t>
+  </si>
+  <si>
+    <t>Biological Sex</t>
+  </si>
+  <si>
+    <t>BIO_SEX</t>
+  </si>
+  <si>
+    <t>ONE_RACE5</t>
   </si>
 </sst>
 </file>
@@ -14410,8 +14422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB5158D-4C91-4CCC-8E26-A99C222AA021}">
   <dimension ref="A1:H124"/>
   <sheetViews>
-    <sheetView topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="H112" sqref="H112"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17495,8 +17507,51 @@
         <v>1614</v>
       </c>
     </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A119" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="C119" s="116" t="s">
+        <v>2050</v>
+      </c>
+      <c r="D119" s="58" t="s">
+        <v>2051</v>
+      </c>
+      <c r="E119" s="49" t="s">
+        <v>1471</v>
+      </c>
+      <c r="F119" s="49" t="s">
+        <v>1364</v>
+      </c>
+      <c r="G119" s="49" t="s">
+        <v>1406</v>
+      </c>
+      <c r="H119" s="49" t="s">
+        <v>2052</v>
+      </c>
+    </row>
     <row r="120" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C120" s="82"/>
+      <c r="A120" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C120" s="82" t="s">
+        <v>2050</v>
+      </c>
+      <c r="D120" s="80" t="s">
+        <v>1362</v>
+      </c>
+      <c r="E120" s="99" t="s">
+        <v>1472</v>
+      </c>
+      <c r="F120" s="74" t="s">
+        <v>19</v>
+      </c>
+      <c r="G120" s="96" t="s">
+        <v>1406</v>
+      </c>
+      <c r="H120" s="21" t="s">
+        <v>2053</v>
+      </c>
     </row>
     <row r="121" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C121" s="82"/>
@@ -17517,7 +17572,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -17525,7 +17581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3F7A32-2A24-9143-AA8A-5502F5BABBAF}">
   <dimension ref="A1:AB230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A206" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A206" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="U218" sqref="U218"/>
     </sheetView>

</xml_diff>

<commit_message>
Adds demographic vars to page 10
</commit_message>
<xml_diff>
--- a/Variables_of_Interest.xlsx
+++ b/Variables_of_Interest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katni\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DB7162-3026-412B-BA9A-ACDE6C725BE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BD25A5-751C-4B8C-A2E2-B4A8FE1E6ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcome Variables" sheetId="2" r:id="rId1"/>
@@ -566,7 +566,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9450" uniqueCount="2054">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9464" uniqueCount="2054">
   <si>
     <t>Wave I</t>
   </si>
@@ -10452,10 +10452,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D83563-E816-4E6C-A07D-139DD8EBC125}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11278,6 +11278,52 @@
       </c>
       <c r="G36" s="58" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="58" t="s">
+        <v>2050</v>
+      </c>
+      <c r="C37" s="58" t="s">
+        <v>2051</v>
+      </c>
+      <c r="D37" s="58" t="s">
+        <v>1471</v>
+      </c>
+      <c r="E37" s="58" t="s">
+        <v>1364</v>
+      </c>
+      <c r="F37" s="58" t="s">
+        <v>1406</v>
+      </c>
+      <c r="G37" s="58" t="s">
+        <v>2052</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="58" t="s">
+        <v>2050</v>
+      </c>
+      <c r="C38" s="58" t="s">
+        <v>1362</v>
+      </c>
+      <c r="D38" s="58" t="s">
+        <v>1472</v>
+      </c>
+      <c r="E38" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" s="58" t="s">
+        <v>1406</v>
+      </c>
+      <c r="G38" s="58" t="s">
+        <v>2053</v>
       </c>
     </row>
   </sheetData>
@@ -14422,7 +14468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB5158D-4C91-4CCC-8E26-A99C222AA021}">
   <dimension ref="A1:H124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+    <sheetView topLeftCell="A94" workbookViewId="0">
       <selection activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixes variables for benchmarks
</commit_message>
<xml_diff>
--- a/Variables_of_Interest.xlsx
+++ b/Variables_of_Interest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katni\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BD25A5-751C-4B8C-A2E2-B4A8FE1E6ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515943F2-4241-4D81-9D06-23D68B203CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcome Variables" sheetId="2" r:id="rId1"/>
@@ -6604,9 +6604,6 @@
     <t>h5id6h</t>
   </si>
   <si>
-    <t>h5cj1d</t>
-  </si>
-  <si>
     <t>h5cj4c</t>
   </si>
   <si>
@@ -6728,6 +6725,9 @@
   </si>
   <si>
     <t>ONE_RACE5</t>
+  </si>
+  <si>
+    <t>h5cj1c</t>
   </si>
 </sst>
 </file>
@@ -10454,8 +10454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D83563-E816-4E6C-A07D-139DD8EBC125}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10501,7 +10501,7 @@
         <v>857</v>
       </c>
       <c r="C2" s="58" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D2" s="58" t="s">
         <v>1471</v>
@@ -10524,7 +10524,7 @@
         <v>857</v>
       </c>
       <c r="C3" s="58" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D3" s="58" t="s">
         <v>1471</v>
@@ -10547,7 +10547,7 @@
         <v>857</v>
       </c>
       <c r="C4" s="58" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D4" s="58" t="s">
         <v>1471</v>
@@ -10570,7 +10570,7 @@
         <v>857</v>
       </c>
       <c r="C5" s="58" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="D5" s="58" t="s">
         <v>1492</v>
@@ -10593,7 +10593,7 @@
         <v>857</v>
       </c>
       <c r="C6" s="58" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="D6" s="58" t="s">
         <v>1471</v>
@@ -10616,7 +10616,7 @@
         <v>857</v>
       </c>
       <c r="C7" s="58" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="D7" s="58" t="s">
         <v>1472</v>
@@ -10639,7 +10639,7 @@
         <v>857</v>
       </c>
       <c r="C8" s="58" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D8" s="58" t="s">
         <v>1515</v>
@@ -10662,7 +10662,7 @@
         <v>857</v>
       </c>
       <c r="C9" s="58" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="D9" s="58" t="s">
         <v>1471</v>
@@ -10685,7 +10685,7 @@
         <v>857</v>
       </c>
       <c r="C10" s="58" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="D10" s="58" t="s">
         <v>1580</v>
@@ -10708,10 +10708,10 @@
         <v>857</v>
       </c>
       <c r="C11" s="58" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="D11" s="58" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
       <c r="E11" s="58" t="s">
         <v>1405</v>
@@ -10731,7 +10731,7 @@
         <v>1999</v>
       </c>
       <c r="C12" s="58" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="D12" s="58" t="s">
         <v>1471</v>
@@ -10751,7 +10751,7 @@
         <v>1999</v>
       </c>
       <c r="C13" s="58" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="D13" s="58" t="s">
         <v>1471</v>
@@ -10774,7 +10774,7 @@
         <v>1999</v>
       </c>
       <c r="C14" s="58" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="D14" s="58" t="s">
         <v>1471</v>
@@ -10794,7 +10794,7 @@
         <v>1999</v>
       </c>
       <c r="C15" s="58" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
       <c r="D15" s="58" t="s">
         <v>1471</v>
@@ -10814,7 +10814,7 @@
         <v>1999</v>
       </c>
       <c r="C16" s="58" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="D16" s="58" t="s">
         <v>1471</v>
@@ -10823,7 +10823,7 @@
         <v>1406</v>
       </c>
       <c r="G16" s="58" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -10834,7 +10834,7 @@
         <v>2000</v>
       </c>
       <c r="C17" s="58" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="D17" s="58" t="s">
         <v>1471</v>
@@ -10843,7 +10843,7 @@
         <v>1406</v>
       </c>
       <c r="G17" s="58" t="s">
-        <v>2012</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -10854,7 +10854,7 @@
         <v>2000</v>
       </c>
       <c r="C18" s="58" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="D18" s="58" t="s">
         <v>1471</v>
@@ -10866,7 +10866,7 @@
         <v>1406</v>
       </c>
       <c r="G18" s="58" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -10877,7 +10877,7 @@
         <v>2000</v>
       </c>
       <c r="C19" s="58" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="D19" s="58" t="s">
         <v>1475</v>
@@ -10889,7 +10889,7 @@
         <v>1408</v>
       </c>
       <c r="G19" s="58" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -10900,7 +10900,7 @@
         <v>2000</v>
       </c>
       <c r="C20" s="58" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="D20" s="58" t="s">
         <v>1516</v>
@@ -10912,7 +10912,7 @@
         <v>1408</v>
       </c>
       <c r="G20" s="58" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -10923,7 +10923,7 @@
         <v>2000</v>
       </c>
       <c r="C21" s="58" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="D21" s="58" t="s">
         <v>1471</v>
@@ -10935,7 +10935,7 @@
         <v>1406</v>
       </c>
       <c r="G21" s="58" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -10946,7 +10946,7 @@
         <v>2000</v>
       </c>
       <c r="C22" s="58" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="D22" s="58" t="s">
         <v>1475</v>
@@ -10958,7 +10958,7 @@
         <v>1408</v>
       </c>
       <c r="G22" s="58" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -10969,7 +10969,7 @@
         <v>2000</v>
       </c>
       <c r="C23" s="58" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="D23" s="58" t="s">
         <v>1496</v>
@@ -10981,7 +10981,7 @@
         <v>1408</v>
       </c>
       <c r="G23" s="58" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -10992,7 +10992,7 @@
         <v>2000</v>
       </c>
       <c r="C24" s="58" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="D24" s="58" t="s">
         <v>1471</v>
@@ -11015,7 +11015,7 @@
         <v>2000</v>
       </c>
       <c r="C25" s="58" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="D25" s="58" t="s">
         <v>1471</v>
@@ -11038,7 +11038,7 @@
         <v>2000</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="D26" s="58" t="s">
         <v>1471</v>
@@ -11061,7 +11061,7 @@
         <v>2001</v>
       </c>
       <c r="C27" s="58" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="D27" s="58" t="s">
         <v>1471</v>
@@ -11070,7 +11070,7 @@
         <v>1406</v>
       </c>
       <c r="G27" s="58" t="s">
-        <v>2012</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -11081,7 +11081,7 @@
         <v>2001</v>
       </c>
       <c r="C28" s="58" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="D28" s="58" t="s">
         <v>1471</v>
@@ -11093,7 +11093,7 @@
         <v>1406</v>
       </c>
       <c r="G28" s="58" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -11104,7 +11104,7 @@
         <v>2001</v>
       </c>
       <c r="C29" s="58" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="D29" s="58" t="s">
         <v>1475</v>
@@ -11116,7 +11116,7 @@
         <v>1408</v>
       </c>
       <c r="G29" s="58" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -11127,7 +11127,7 @@
         <v>2001</v>
       </c>
       <c r="C30" s="58" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="D30" s="58" t="s">
         <v>1516</v>
@@ -11139,7 +11139,7 @@
         <v>1408</v>
       </c>
       <c r="G30" s="58" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -11150,7 +11150,7 @@
         <v>2001</v>
       </c>
       <c r="C31" s="58" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="D31" s="58" t="s">
         <v>1471</v>
@@ -11162,7 +11162,7 @@
         <v>1406</v>
       </c>
       <c r="G31" s="58" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -11173,7 +11173,7 @@
         <v>2001</v>
       </c>
       <c r="C32" s="58" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="D32" s="58" t="s">
         <v>1475</v>
@@ -11185,7 +11185,7 @@
         <v>1408</v>
       </c>
       <c r="G32" s="58" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -11196,7 +11196,7 @@
         <v>2001</v>
       </c>
       <c r="C33" s="58" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="D33" s="58" t="s">
         <v>1496</v>
@@ -11208,7 +11208,7 @@
         <v>1408</v>
       </c>
       <c r="G33" s="58" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -11219,7 +11219,7 @@
         <v>2001</v>
       </c>
       <c r="C34" s="58" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="D34" s="58" t="s">
         <v>1471</v>
@@ -11242,7 +11242,7 @@
         <v>2001</v>
       </c>
       <c r="C35" s="58" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="D35" s="58" t="s">
         <v>1471</v>
@@ -11265,7 +11265,7 @@
         <v>2001</v>
       </c>
       <c r="C36" s="58" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="D36" s="58" t="s">
         <v>1471</v>
@@ -11285,10 +11285,10 @@
         <v>0</v>
       </c>
       <c r="B37" s="58" t="s">
+        <v>2049</v>
+      </c>
+      <c r="C37" s="58" t="s">
         <v>2050</v>
-      </c>
-      <c r="C37" s="58" t="s">
-        <v>2051</v>
       </c>
       <c r="D37" s="58" t="s">
         <v>1471</v>
@@ -11300,7 +11300,7 @@
         <v>1406</v>
       </c>
       <c r="G37" s="58" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -11308,7 +11308,7 @@
         <v>4</v>
       </c>
       <c r="B38" s="58" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="C38" s="58" t="s">
         <v>1362</v>
@@ -11323,7 +11323,7 @@
         <v>1406</v>
       </c>
       <c r="G38" s="58" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
     </row>
   </sheetData>
@@ -11698,7 +11698,7 @@
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U46" sqref="U46"/>
+      <selection pane="topRight" activeCell="U62" sqref="U62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13644,7 +13644,7 @@
         <v>1406</v>
       </c>
       <c r="U45" s="29" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="47" spans="1:28" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -14016,7 +14016,7 @@
         <v>1406</v>
       </c>
       <c r="U54" s="20" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="V54" s="20"/>
       <c r="W54" s="20"/>
@@ -14469,7 +14469,7 @@
   <dimension ref="A1:H124"/>
   <sheetViews>
     <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D120" sqref="D120"/>
+      <selection activeCell="H118" sqref="H118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17368,7 +17368,7 @@
         <v>1406</v>
       </c>
       <c r="H111" s="48" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="112" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -17446,7 +17446,7 @@
         <v>1406</v>
       </c>
       <c r="H114" s="21" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="115" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -17558,10 +17558,10 @@
         <v>0</v>
       </c>
       <c r="C119" s="116" t="s">
+        <v>2049</v>
+      </c>
+      <c r="D119" s="58" t="s">
         <v>2050</v>
-      </c>
-      <c r="D119" s="58" t="s">
-        <v>2051</v>
       </c>
       <c r="E119" s="49" t="s">
         <v>1471</v>
@@ -17573,7 +17573,7 @@
         <v>1406</v>
       </c>
       <c r="H119" s="49" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="120" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -17581,7 +17581,7 @@
         <v>4</v>
       </c>
       <c r="C120" s="82" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="D120" s="80" t="s">
         <v>1362</v>
@@ -17596,7 +17596,7 @@
         <v>1406</v>
       </c>
       <c r="H120" s="21" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="121" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -23816,7 +23816,7 @@
         <v>1406</v>
       </c>
       <c r="P225" s="20" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="226" spans="1:24" x14ac:dyDescent="0.3">
@@ -28073,7 +28073,7 @@
         <v>1406</v>
       </c>
       <c r="H161" s="21" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.3">
@@ -30869,7 +30869,7 @@
         <v>1406</v>
       </c>
       <c r="H269" s="21" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
     </row>
     <row r="270" spans="1:8" x14ac:dyDescent="0.3">
@@ -30895,7 +30895,7 @@
         <v>1406</v>
       </c>
       <c r="H270" s="21" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.3">
@@ -30921,7 +30921,7 @@
         <v>1406</v>
       </c>
       <c r="H271" s="21" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
     </row>
     <row r="272" spans="1:8" x14ac:dyDescent="0.3">
@@ -30947,7 +30947,7 @@
         <v>1406</v>
       </c>
       <c r="H272" s="21" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="273" spans="1:8" x14ac:dyDescent="0.3">
@@ -30973,7 +30973,7 @@
         <v>1406</v>
       </c>
       <c r="H273" s="21" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="274" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>